<commit_message>
0.kattan da çağrı alıyor
</commit_message>
<xml_diff>
--- a/elevator_simulation/bin/Debug/net8.0-windows/ml_training_data.xlsx
+++ b/elevator_simulation/bin/Debug/net8.0-windows/ml_training_data.xlsx
@@ -83,6 +83,21 @@
   </x:si>
   <x:si>
     <x:t>18:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07:58:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:58:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>05:52:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2026-01-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23:45:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2124,6 +2139,1717 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
+    <x:row r="58" spans="1:9">
+      <x:c r="A58" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B58" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C58" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D58" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E58" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F58" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G58" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H58" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I58" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:9">
+      <x:c r="A59" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C59" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D59" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E59" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F59" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G59" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H59" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I59" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:9">
+      <x:c r="A60" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B60" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C60" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D60" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E60" s="2">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F60" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G60" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H60" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I60" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:9">
+      <x:c r="A61" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C61" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D61" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E61" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F61" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G61" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H61" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I61" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:9">
+      <x:c r="A62" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B62" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C62" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D62" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E62" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F62" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G62" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H62" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I62" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:9">
+      <x:c r="A63" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C63" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D63" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E63" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F63" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G63" s="0">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H63" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I63" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:9">
+      <x:c r="A64" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B64" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C64" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D64" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E64" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F64" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G64" s="2">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H64" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="I64" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:9">
+      <x:c r="A65" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C65" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D65" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E65" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F65" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G65" s="0">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="H65" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I65" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:9">
+      <x:c r="A66" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B66" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C66" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D66" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E66" s="2">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F66" s="2">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G66" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H66" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I66" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:9">
+      <x:c r="A67" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C67" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D67" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E67" s="0">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F67" s="0">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G67" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H67" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I67" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:9">
+      <x:c r="A68" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B68" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C68" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D68" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E68" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F68" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G68" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H68" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I68" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:9">
+      <x:c r="A69" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C69" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D69" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E69" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F69" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G69" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H69" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I69" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:9">
+      <x:c r="A70" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B70" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C70" s="2">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D70" s="2">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E70" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F70" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G70" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H70" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I70" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:9">
+      <x:c r="A71" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C71" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D71" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E71" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F71" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G71" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H71" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I71" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:9">
+      <x:c r="A72" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B72" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C72" s="2">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D72" s="2">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E72" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F72" s="2">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G72" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H72" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I72" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:9">
+      <x:c r="A73" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C73" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D73" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E73" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F73" s="0">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G73" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H73" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I73" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:9">
+      <x:c r="A74" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B74" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C74" s="2">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D74" s="2">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E74" s="2">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F74" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G74" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H74" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I74" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:9">
+      <x:c r="A75" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C75" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D75" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E75" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F75" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G75" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H75" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I75" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:9">
+      <x:c r="A76" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B76" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C76" s="2">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D76" s="2">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E76" s="2">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F76" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G76" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H76" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I76" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:9">
+      <x:c r="A77" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C77" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D77" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E77" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F77" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G77" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H77" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I77" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:9">
+      <x:c r="A78" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B78" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C78" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D78" s="2">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E78" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F78" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G78" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H78" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I78" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:9">
+      <x:c r="A79" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C79" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D79" s="0">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E79" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F79" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G79" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H79" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I79" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:9">
+      <x:c r="A80" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B80" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C80" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D80" s="2">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E80" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F80" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G80" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H80" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I80" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:9">
+      <x:c r="A81" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C81" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D81" s="0">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E81" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F81" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G81" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H81" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I81" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:9">
+      <x:c r="A82" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B82" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C82" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D82" s="2">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E82" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F82" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G82" s="2">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H82" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I82" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:9">
+      <x:c r="A83" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C83" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D83" s="0">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E83" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F83" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G83" s="0">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H83" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="I83" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:9">
+      <x:c r="A84" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B84" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C84" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D84" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E84" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F84" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G84" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H84" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I84" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:9">
+      <x:c r="A85" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C85" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D85" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E85" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F85" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G85" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H85" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I85" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:9">
+      <x:c r="A86" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B86" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C86" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D86" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E86" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F86" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G86" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H86" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I86" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:9">
+      <x:c r="A87" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C87" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D87" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E87" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F87" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G87" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H87" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I87" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:9">
+      <x:c r="A88" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B88" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C88" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D88" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E88" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F88" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G88" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H88" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I88" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:9">
+      <x:c r="A89" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C89" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D89" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E89" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F89" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G89" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H89" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I89" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:9">
+      <x:c r="A90" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B90" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C90" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D90" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E90" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F90" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G90" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H90" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I90" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:9">
+      <x:c r="A91" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C91" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E91" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G91" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I91" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:9">
+      <x:c r="A92" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B92" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C92" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D92" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E92" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F92" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G92" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H92" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I92" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:9">
+      <x:c r="A93" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C93" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E93" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G93" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I93" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:9">
+      <x:c r="A94" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B94" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C94" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D94" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E94" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F94" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G94" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H94" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I94" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:9">
+      <x:c r="A95" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C95" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E95" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F95" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I95" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:9">
+      <x:c r="A96" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B96" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C96" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D96" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E96" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F96" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G96" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H96" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I96" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:9">
+      <x:c r="A97" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C97" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E97" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F97" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I97" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:9">
+      <x:c r="A98" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B98" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C98" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D98" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E98" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F98" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G98" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H98" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I98" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:9">
+      <x:c r="A99" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C99" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D99" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E99" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F99" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G99" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H99" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I99" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:9">
+      <x:c r="A100" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B100" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C100" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D100" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E100" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F100" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G100" s="2">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H100" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I100" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:9">
+      <x:c r="A101" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C101" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D101" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E101" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F101" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G101" s="0">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H101" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="I101" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:9">
+      <x:c r="A102" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B102" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C102" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D102" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E102" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F102" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G102" s="2">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="H102" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="I102" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:9">
+      <x:c r="A103" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C103" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D103" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E103" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F103" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G103" s="0">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="H103" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="I103" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:9">
+      <x:c r="A104" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B104" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C104" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D104" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E104" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F104" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G104" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H104" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I104" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:9">
+      <x:c r="A105" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C105" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D105" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E105" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F105" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G105" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H105" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I105" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:9">
+      <x:c r="A106" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B106" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C106" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D106" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E106" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F106" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G106" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H106" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I106" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:9">
+      <x:c r="A107" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C107" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E107" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I107" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:9">
+      <x:c r="A108" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B108" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C108" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D108" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E108" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F108" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G108" s="2">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H108" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I108" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:9">
+      <x:c r="A109" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C109" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E109" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I109" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:9">
+      <x:c r="A110" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B110" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C110" s="2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D110" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E110" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F110" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G110" s="2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H110" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I110" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:9">
+      <x:c r="A111" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C111" s="0">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D111" s="0">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I111" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:9">
+      <x:c r="A112" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B112" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C112" s="2">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D112" s="2">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E112" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F112" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G112" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H112" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I112" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:9">
+      <x:c r="A113" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C113" s="0">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D113" s="0">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E113" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F113" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G113" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H113" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I113" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:9">
+      <x:c r="A114" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B114" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C114" s="2">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D114" s="2">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E114" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F114" s="2">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G114" s="2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H114" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I114" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:9">
+      <x:c r="A115" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C115" s="0">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D115" s="0">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E115" s="0">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F115" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G115" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H115" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I115" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:9">
+      <x:c r="A116" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B116" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C116" s="2">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D116" s="2">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E116" s="2">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F116" s="2">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G116" s="2">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H116" s="2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I116" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>